<commit_message>
MinX parameter files update
</commit_message>
<xml_diff>
--- a/Parameters/country_parameters.xlsx
+++ b/Parameters/country_parameters.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\engs1825\Documents\GitHub\GeoH2\Parameters\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4EAA8322-40EE-405B-A30E-B0059B6B7951}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7489AB1B-4E01-4B10-995A-DFD1D94E7843}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17640" xr2:uid="{60BD1E41-9A81-F547-A629-52DD9269BE2D}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{60BD1E41-9A81-F547-A629-52DD9269BE2D}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="16">
   <si>
     <t>Country</t>
   </si>
@@ -79,6 +79,9 @@
   </si>
   <si>
     <t>Diesel price (euros/kWh)</t>
+  </si>
+  <si>
+    <t>Grid connection cost (euros/kW)</t>
   </si>
 </sst>
 </file>
@@ -437,10 +440,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1A655327-FB0F-D040-A870-A9F18A82B881}">
-  <dimension ref="A1:L4"/>
+  <dimension ref="A1:M4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C1" sqref="C1"/>
+    <sheetView tabSelected="1" topLeftCell="E1" workbookViewId="0">
+      <selection activeCell="M5" sqref="M5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -457,7 +460,7 @@
     <col min="11" max="11" width="17" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -494,8 +497,11 @@
       <c r="L1" t="s">
         <v>10</v>
       </c>
+      <c r="M1" t="s">
+        <v>15</v>
+      </c>
     </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>11</v>
       </c>
@@ -532,8 +538,11 @@
       <c r="L2">
         <v>50</v>
       </c>
+      <c r="M2">
+        <v>150</v>
+      </c>
     </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>12</v>
       </c>
@@ -570,8 +579,11 @@
       <c r="L3">
         <v>50</v>
       </c>
+      <c r="M3">
+        <v>150</v>
+      </c>
     </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>13</v>
       </c>
@@ -607,6 +619,9 @@
       </c>
       <c r="L4">
         <v>50</v>
+      </c>
+      <c r="M4">
+        <v>150</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
rail transport and grid construction
</commit_message>
<xml_diff>
--- a/Parameters/country_parameters.xlsx
+++ b/Parameters/country_parameters.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\engs1825\Documents\GitHub\GeoH2\Parameters\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7489AB1B-4E01-4B10-995A-DFD1D94E7843}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D24FBB07-83C1-4FAD-8F8D-9406E7832452}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{60BD1E41-9A81-F547-A629-52DD9269BE2D}"/>
   </bookViews>
@@ -442,25 +442,25 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1A655327-FB0F-D040-A870-A9F18A82B881}">
   <dimension ref="A1:M4"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E1" workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="M5" sqref="M5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="14.875" customWidth="1"/>
-    <col min="2" max="3" width="24.625" customWidth="1"/>
-    <col min="4" max="4" width="24.375" customWidth="1"/>
-    <col min="5" max="5" width="19.625" customWidth="1"/>
+    <col min="1" max="1" width="14.8984375" customWidth="1"/>
+    <col min="2" max="3" width="24.59765625" customWidth="1"/>
+    <col min="4" max="4" width="24.3984375" customWidth="1"/>
+    <col min="5" max="5" width="19.59765625" customWidth="1"/>
     <col min="6" max="6" width="22" customWidth="1"/>
-    <col min="7" max="7" width="26.125" customWidth="1"/>
-    <col min="8" max="8" width="19.875" customWidth="1"/>
-    <col min="9" max="9" width="20.125" customWidth="1"/>
-    <col min="10" max="10" width="18.125" customWidth="1"/>
+    <col min="7" max="7" width="26.09765625" customWidth="1"/>
+    <col min="8" max="8" width="19.8984375" customWidth="1"/>
+    <col min="9" max="9" width="20.09765625" customWidth="1"/>
+    <col min="10" max="10" width="18.09765625" customWidth="1"/>
     <col min="11" max="11" width="17" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -501,7 +501,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="2" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>11</v>
       </c>
@@ -542,7 +542,7 @@
         <v>150</v>
       </c>
     </row>
-    <row r="3" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>12</v>
       </c>
@@ -583,7 +583,7 @@
         <v>150</v>
       </c>
     </row>
-    <row r="4" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>13</v>
       </c>

</xml_diff>